<commit_message>
WPT experiment data and presentation about usage of data and fig
in the journals
</commit_message>
<xml_diff>
--- a/WPT/Testler/Inductance Matrices.xlsx
+++ b/WPT/Testler/Inductance Matrices.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9D2933-E120-4788-89C6-C986E21BCBC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010E50A8-1AE8-4B08-87B9-B9016FA28153}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -868,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17AC5B0D-928A-4DBD-A5ED-965B8572B295}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="A1:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -913,7 +913,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>177</v>
+        <v>177.5</v>
       </c>
       <c r="C3" s="1">
         <v>65.599999999999994</v>
@@ -927,7 +927,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>178</v>
+        <v>177.5</v>
       </c>
       <c r="C4" s="1">
         <v>124.85</v>
@@ -983,7 +983,7 @@
       </c>
       <c r="B9" s="1">
         <f>(B3-B2-C3)/2</f>
-        <v>13.950000000000003</v>
+        <v>14.200000000000003</v>
       </c>
       <c r="C9" s="1">
         <f>C3</f>
@@ -999,7 +999,7 @@
       </c>
       <c r="B10" s="1">
         <f>(B4-B2-D4)/2</f>
-        <v>14.549999999999997</v>
+        <v>14.299999999999997</v>
       </c>
       <c r="C10" s="1">
         <f>(C4-C3-D4)/2</f>
@@ -1069,7 +1069,7 @@
       </c>
       <c r="B17" s="1">
         <f>B9/SQRT(B8*C9)</f>
-        <v>0.1884859792238007</v>
+        <v>0.19186386415612688</v>
       </c>
       <c r="C17" s="1">
         <f>1</f>
@@ -1085,7 +1085,7 @@
       </c>
       <c r="B18" s="1">
         <f>B10/SQRT(D10*B8)</f>
-        <v>0.19689327436422069</v>
+        <v>0.19351022841294543</v>
       </c>
       <c r="C18" s="1">
         <f>C10/SQRT(C9*D10)</f>
@@ -1105,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{237FD467-88B6-43FC-A84D-8A17D23D16E7}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>